<commit_message>
moving towards a final version'
</commit_message>
<xml_diff>
--- a/data/TablesZhangetal2017_11_28_EN_21.xlsx
+++ b/data/TablesZhangetal2017_11_28_EN_21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rver4657\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200BB12C-7034-4D2D-AE06-951E66B819D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2F1CC1-B453-4DF5-A60E-6A712E828C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="3" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5214" uniqueCount="949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5221" uniqueCount="951">
   <si>
     <t>Watershed #</t>
   </si>
@@ -2978,6 +2978,12 @@
   </si>
   <si>
     <t>Pitman 1978 from Filoso et al. 2017</t>
+  </si>
+  <si>
+    <t>Valtorto</t>
+  </si>
+  <si>
+    <t>Stoof et al. 2012 https://hess.copernicus.org/articles/16/267/2012/. Rainfall and Et calculated as the average of the reported data in Table 3 in the paper</t>
   </si>
 </sst>
 </file>
@@ -3354,13 +3360,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3372,13 +3381,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -20706,7 +20712,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="252" spans="1:19" ht="39.4" thickBot="1">
+    <row r="252" spans="1:19" ht="49.15" thickBot="1">
       <c r="A252" s="55">
         <v>312</v>
       </c>
@@ -35820,10 +35826,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD75620-6F76-4BA6-A94E-CE93109D006F}">
-  <dimension ref="A1:V46"/>
+  <dimension ref="A1:V47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="S47" sqref="S47"/>
+      <selection activeCell="O46" sqref="O46:O47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -35837,34 +35843,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="76" t="s">
+      <c r="E1" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="76" t="s">
+      <c r="F1" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="74" t="s">
+      <c r="H1" s="75" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="76" t="s">
+      <c r="J1" s="70" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="72" t="s">
@@ -35885,16 +35891,16 @@
       <c r="P1" s="72" t="s">
         <v>541</v>
       </c>
-      <c r="Q1" s="70" t="s">
+      <c r="Q1" s="77" t="s">
         <v>683</v>
       </c>
-      <c r="R1" s="70" t="s">
+      <c r="R1" s="77" t="s">
         <v>684</v>
       </c>
-      <c r="S1" s="71" t="s">
+      <c r="S1" s="78" t="s">
         <v>918</v>
       </c>
-      <c r="T1" s="71" t="s">
+      <c r="T1" s="78" t="s">
         <v>776</v>
       </c>
       <c r="U1" s="64" t="s">
@@ -35902,26 +35908,26 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="28.5" customHeight="1" thickBot="1">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
       <c r="U2" s="68" t="s">
         <v>916</v>
       </c>
@@ -37633,7 +37639,7 @@
         <v>-83.214777799999993</v>
       </c>
       <c r="O31">
-        <f t="shared" ref="O31:O46" si="0">R31-Q31</f>
+        <f t="shared" ref="O31:O47" si="0">R31-Q31</f>
         <v>71</v>
       </c>
       <c r="Q31">
@@ -38413,20 +38419,65 @@
         <v>566</v>
       </c>
     </row>
+    <row r="47" spans="1:19">
+      <c r="A47">
+        <v>223</v>
+      </c>
+      <c r="B47" t="s">
+        <v>949</v>
+      </c>
+      <c r="C47">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="D47">
+        <f>SUM(1/(199/365)*878,1352,1/(265/365)*1069,1568)/4</f>
+        <v>1500.6995591163363</v>
+      </c>
+      <c r="E47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47">
+        <v>-100</v>
+      </c>
+      <c r="H47">
+        <v>60</v>
+      </c>
+      <c r="I47" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" t="s">
+        <v>16</v>
+      </c>
+      <c r="K47" t="s">
+        <v>950</v>
+      </c>
+      <c r="L47">
+        <f>40+6/60+21/3600</f>
+        <v>40.105833333333337</v>
+      </c>
+      <c r="M47">
+        <f>8+7/60+3/3600</f>
+        <v>8.1174999999999997</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Q47">
+        <v>2008</v>
+      </c>
+      <c r="R47">
+        <v>2010</v>
+      </c>
+      <c r="S47" t="s">
+        <v>566</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="T1:T2"/>
@@ -38435,6 +38486,18 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>